<commit_message>
Neue Pakete in den Demos
</commit_message>
<xml_diff>
--- a/results/AllApps_ConsolidatedReport.xlsx
+++ b/results/AllApps_ConsolidatedReport.xlsx
@@ -23,6 +23,18 @@
     <x:t>PackageName</x:t>
   </x:si>
   <x:si>
+    <x:t>FromVersion</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ToVersion</x:t>
+  </x:si>
+  <x:si>
+    <x:t>FromLicense</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ToLicense</x:t>
+  </x:si>
+  <x:si>
     <x:t>HighestVersion</x:t>
   </x:si>
   <x:si>
@@ -32,19 +44,61 @@
     <x:t>LicenseUrl</x:t>
   </x:si>
   <x:si>
+    <x:t>HasVersionChange</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HasLicenseChange</x:t>
+  </x:si>
+  <x:si>
     <x:t>nuget</x:t>
   </x:si>
   <x:si>
+    <x:t>Microsoft.AspNetCore.SpaServices.Extensions</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8.0.23</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MIT</x:t>
+  </x:si>
+  <x:si>
+    <x:t/>
+  </x:si>
+  <x:si>
+    <x:t>No</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Microsoft.Extensions.FileProviders.Abstractions</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8.0.0</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Microsoft.Extensions.FileProviders.Physical</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Microsoft.Extensions.FileSystemGlobbing</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Microsoft.Extensions.Primitives</x:t>
+  </x:si>
+  <x:si>
     <x:t>Newtonsoft.Json</x:t>
   </x:si>
   <x:si>
     <x:t>13.0.4</x:t>
   </x:si>
   <x:si>
-    <x:t>MIT</x:t>
-  </x:si>
-  <x:si>
-    <x:t/>
+    <x:t>13.0.0</x:t>
+  </x:si>
+  <x:si>
+    <x:t>UNKNOWN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.nuget.org/packages/Newtonsoft.Json/13.0.0</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Yes</x:t>
   </x:si>
   <x:si>
     <x:t>App</x:t>
@@ -53,16 +107,10 @@
     <x:t>ChangeType</x:t>
   </x:si>
   <x:si>
-    <x:t>FromVersion</x:t>
-  </x:si>
-  <x:si>
-    <x:t>FromLicense</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ToVersion</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ToLicense</x:t>
+    <x:t>NugetDemo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LicenseChanged</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -72,7 +120,7 @@
   <x:numFmts count="1">
     <x:numFmt numFmtId="0" formatCode=""/>
   </x:numFmts>
-  <x:fonts count="2">
+  <x:fonts count="3">
     <x:font>
       <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
@@ -85,6 +133,14 @@
       <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
       <x:color rgb="FFFFFFFF"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:u val="single"/>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF0000FF"/>
       <x:name val="Calibri"/>
       <x:family val="2"/>
     </x:font>
@@ -121,21 +177,28 @@
       </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="2">
+  <x:cellStyleXfs count="3">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="2">
+  <x:cellXfs count="3">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellXfs>
@@ -433,20 +496,26 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:E2"/>
+  <x:dimension ref="A1:K7"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
     <x:col min="1" max="1" width="16.282054" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="15.996339" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="14.424911" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="7.424911" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="9.853482" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="44.139196" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="12.567768" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="9.853482" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="11.996339" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="10.853482" style="0" customWidth="1"/>
+    <x:col min="7" max="7" width="14.424911" style="0" customWidth="1"/>
+    <x:col min="8" max="8" width="10.853482" style="0" customWidth="1"/>
+    <x:col min="9" max="9" width="53.996339" style="0" customWidth="1"/>
+    <x:col min="10" max="10" width="17.853482" style="0" customWidth="1"/>
+    <x:col min="11" max="11" width="17.567768" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:5" s="1" customFormat="1">
+    <x:row r="1" spans="1:11" s="1" customFormat="1">
       <x:c r="A1" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -462,25 +531,239 @@
       <x:c r="E1" s="1" t="s">
         <x:v>4</x:v>
       </x:c>
+      <x:c r="F1" s="1" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="G1" s="1" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H1" s="1" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I1" s="1" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="J1" s="1" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="K1" s="1" t="s">
+        <x:v>10</x:v>
+      </x:c>
     </x:row>
-    <x:row r="2" spans="1:5">
+    <x:row r="2" spans="1:11">
       <x:c r="A2" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="D2" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E2" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F2" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G2" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H2" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I2" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="J2" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="K2" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:11">
+      <x:c r="A3" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F3" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G3" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="H3" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I3" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="J3" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="K3" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:11">
+      <x:c r="A4" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F4" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G4" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="H4" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I4" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="J4" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="K4" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:11">
+      <x:c r="A5" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F5" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G5" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="H5" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I5" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="J5" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="K5" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:11">
+      <x:c r="A6" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="E6" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F6" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G6" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="H6" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I6" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="J6" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="K6" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:11">
+      <x:c r="A7" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="E7" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F7" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="G7" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H7" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="I7" s="2" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="J7" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="K7" s="0" t="s">
+        <x:v>27</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
+  <x:hyperlinks>
+    <x:hyperlink ref="I7" r:id="rId6"/>
+  </x:hyperlinks>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
@@ -494,26 +777,26 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:I1"/>
+  <x:dimension ref="A1:I2"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="4.424911" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="11.567768" style="0" customWidth="1"/>
     <x:col min="2" max="2" width="16.282054" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="13.567768" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="11.853482" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="15.996339" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="15.282054" style="0" customWidth="1"/>
     <x:col min="5" max="5" width="12.567768" style="0" customWidth="1"/>
     <x:col min="6" max="6" width="11.996339" style="0" customWidth="1"/>
     <x:col min="7" max="7" width="9.853482" style="0" customWidth="1"/>
-    <x:col min="8" max="8" width="9.567768" style="0" customWidth="1"/>
+    <x:col min="8" max="8" width="10.853482" style="0" customWidth="1"/>
     <x:col min="9" max="9" width="9.853482" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:9" s="1" customFormat="1">
       <x:c r="A1" s="1" t="s">
-        <x:v>10</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="B1" s="1" t="s">
         <x:v>0</x:v>
@@ -522,22 +805,51 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="D1" s="1" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="E1" s="1" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="F1" s="1" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="G1" s="1" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="H1" s="1" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="I1" s="1" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:9">
+      <x:c r="A2" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="E1" s="1" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="F1" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="G1" s="1" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="H1" s="1" t="s">
+      <x:c r="C2" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="E2" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="F2" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G2" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H2" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="I2" s="0" t="s">
         <x:v>15</x:v>
-      </x:c>
-      <x:c r="I1" s="1" t="s">
-        <x:v>4</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Versions und Lizenzänderungen Test
</commit_message>
<xml_diff>
--- a/results/AllApps_ConsolidatedReport.xlsx
+++ b/results/AllApps_ConsolidatedReport.xlsx
@@ -50,24 +50,84 @@
     <x:t>HasLicenseChange</x:t>
   </x:si>
   <x:si>
+    <x:t>npm</x:t>
+  </x:si>
+  <x:si>
+    <x:t>js-tokens</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4.0.0</x:t>
+  </x:si>
+  <x:si>
+    <x:t>UNKNOWN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.npmjs.com/package/js-tokens</x:t>
+  </x:si>
+  <x:si>
+    <x:t>No</x:t>
+  </x:si>
+  <x:si>
+    <x:t>loose-envify</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.4.0</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.npmjs.com/package/loose-envify</x:t>
+  </x:si>
+  <x:si>
+    <x:t>react</x:t>
+  </x:si>
+  <x:si>
+    <x:t>18.2.0</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.npmjs.com/package/react</x:t>
+  </x:si>
+  <x:si>
     <x:t>nuget</x:t>
   </x:si>
   <x:si>
+    <x:t>ClosedXML</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0.105.0</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MIT</x:t>
+  </x:si>
+  <x:si>
+    <x:t/>
+  </x:si>
+  <x:si>
+    <x:t>ClosedXML.Parser</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2.0.0</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DocumentFormat.OpenXml</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3.1.1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DocumentFormat.OpenXml.Framework</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ExcelNumberFormat</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.1.0</x:t>
+  </x:si>
+  <x:si>
     <x:t>Microsoft.AspNetCore.SpaServices.Extensions</x:t>
   </x:si>
   <x:si>
     <x:t>8.0.23</x:t>
   </x:si>
   <x:si>
-    <x:t>MIT</x:t>
-  </x:si>
-  <x:si>
-    <x:t/>
-  </x:si>
-  <x:si>
-    <x:t>No</x:t>
-  </x:si>
-  <x:si>
     <x:t>Microsoft.Extensions.FileProviders.Abstractions</x:t>
   </x:si>
   <x:si>
@@ -86,31 +146,52 @@
     <x:t>Newtonsoft.Json</x:t>
   </x:si>
   <x:si>
-    <x:t>13.0.4</x:t>
-  </x:si>
-  <x:si>
     <x:t>13.0.0</x:t>
   </x:si>
   <x:si>
-    <x:t>UNKNOWN</x:t>
-  </x:si>
-  <x:si>
     <x:t>https://www.nuget.org/packages/Newtonsoft.Json/13.0.0</x:t>
   </x:si>
   <x:si>
-    <x:t>Yes</x:t>
+    <x:t>Node.js</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0.12.7</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://raw.github.com/joyent/node/v0.12.7/LICENSE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NoGit</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0.1.0</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Npm</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3.5.2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://raw.githubusercontent.com/npm/npm/v3.5.2/LICENSE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RBush.Signed</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SixLabors.Fonts</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.0.0</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Apache-2.0</x:t>
   </x:si>
   <x:si>
     <x:t>App</x:t>
   </x:si>
   <x:si>
     <x:t>ChangeType</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NugetDemo</x:t>
-  </x:si>
-  <x:si>
-    <x:t>LicenseChanged</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -496,7 +577,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:K7"/>
+  <x:dimension ref="A1:K20"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -510,7 +591,7 @@
     <x:col min="6" max="6" width="10.853482" style="0" customWidth="1"/>
     <x:col min="7" max="7" width="14.424911" style="0" customWidth="1"/>
     <x:col min="8" max="8" width="10.853482" style="0" customWidth="1"/>
-    <x:col min="9" max="9" width="53.996339" style="0" customWidth="1"/>
+    <x:col min="9" max="9" width="58.424911" style="0" customWidth="1"/>
     <x:col min="10" max="10" width="17.853482" style="0" customWidth="1"/>
     <x:col min="11" max="11" width="17.567768" style="0" customWidth="1"/>
   </x:cols>
@@ -575,7 +656,7 @@
       <x:c r="H2" s="0" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="I2" s="0" t="s">
+      <x:c r="I2" s="2" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="J2" s="0" t="s">
@@ -610,8 +691,8 @@
       <x:c r="H3" s="0" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="I3" s="0" t="s">
-        <x:v>15</x:v>
+      <x:c r="I3" s="2" t="s">
+        <x:v>19</x:v>
       </x:c>
       <x:c r="J3" s="0" t="s">
         <x:v>16</x:v>
@@ -625,13 +706,13 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="D4" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E4" s="0" t="s">
         <x:v>14</x:v>
@@ -640,13 +721,13 @@
         <x:v>14</x:v>
       </x:c>
       <x:c r="G4" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="H4" s="0" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="I4" s="0" t="s">
-        <x:v>15</x:v>
+      <x:c r="I4" s="2" t="s">
+        <x:v>22</x:v>
       </x:c>
       <x:c r="J4" s="0" t="s">
         <x:v>16</x:v>
@@ -657,31 +738,31 @@
     </x:row>
     <x:row r="5" spans="1:11">
       <x:c r="A5" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="E5" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="F5" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="G5" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="H5" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="I5" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="J5" s="0" t="s">
         <x:v>16</x:v>
@@ -692,31 +773,31 @@
     </x:row>
     <x:row r="6" spans="1:11">
       <x:c r="A6" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="E6" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="F6" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="G6" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="H6" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="I6" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="J6" s="0" t="s">
         <x:v>16</x:v>
@@ -727,42 +808,502 @@
     </x:row>
     <x:row r="7" spans="1:11">
       <x:c r="A7" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="E7" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="F7" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="G7" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="H7" s="0" t="s">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="I7" s="2" t="s">
-        <x:v>26</x:v>
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="I7" s="0" t="s">
+        <x:v>27</x:v>
       </x:c>
       <x:c r="J7" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="K7" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:11">
+      <x:c r="A8" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="E8" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="F8" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="G8" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="H8" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="I8" s="0" t="s">
         <x:v>27</x:v>
       </x:c>
-      <x:c r="K7" s="0" t="s">
+      <x:c r="J8" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="K8" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:11">
+      <x:c r="A9" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="E9" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="F9" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="G9" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="H9" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="I9" s="0" t="s">
         <x:v>27</x:v>
+      </x:c>
+      <x:c r="J9" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="K9" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:11">
+      <x:c r="A10" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="C10" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="D10" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="E10" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="F10" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="G10" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="H10" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="I10" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="J10" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="K10" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:11">
+      <x:c r="A11" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="C11" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="D11" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="E11" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="F11" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="G11" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="H11" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="I11" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="J11" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="K11" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:11">
+      <x:c r="A12" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B12" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="C12" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="D12" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="E12" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="F12" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="G12" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="H12" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="I12" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="J12" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="K12" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:11">
+      <x:c r="A13" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="C13" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="D13" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="E13" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="F13" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="G13" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="H13" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="I13" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="J13" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="K13" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:11">
+      <x:c r="A14" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B14" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="C14" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="D14" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="E14" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="F14" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="G14" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="H14" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="I14" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="J14" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="K14" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:11">
+      <x:c r="A15" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B15" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="C15" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="D15" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="E15" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F15" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G15" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="H15" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I15" s="2" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="J15" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="K15" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:11">
+      <x:c r="A16" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B16" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="C16" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="D16" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="E16" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F16" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G16" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="H16" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I16" s="2" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="J16" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="K16" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:11">
+      <x:c r="A17" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B17" s="0" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="C17" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="D17" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="E17" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F17" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G17" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="H17" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I17" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="J17" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="K17" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:11">
+      <x:c r="A18" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B18" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="C18" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="D18" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="E18" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F18" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G18" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="H18" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I18" s="2" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="J18" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="K18" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:11">
+      <x:c r="A19" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B19" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="C19" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D19" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="E19" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="F19" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="G19" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H19" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="I19" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="J19" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="K19" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:11">
+      <x:c r="A20" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B20" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="C20" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="D20" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="E20" s="0" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="F20" s="0" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="G20" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="H20" s="0" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="I20" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="J20" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="K20" s="0" t="s">
+        <x:v>16</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
   <x:hyperlinks>
-    <x:hyperlink ref="I7" r:id="rId6"/>
+    <x:hyperlink ref="I2" r:id="rId6"/>
+    <x:hyperlink ref="I3" r:id="rId7"/>
+    <x:hyperlink ref="I4" r:id="rId8"/>
+    <x:hyperlink ref="I15" r:id="rId9"/>
+    <x:hyperlink ref="I16" r:id="rId10"/>
+    <x:hyperlink ref="I18" r:id="rId11"/>
   </x:hyperlinks>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
@@ -777,26 +1318,26 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:I2"/>
+  <x:dimension ref="A1:I1"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="11.567768" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="4.424911" style="0" customWidth="1"/>
     <x:col min="2" max="2" width="16.282054" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="15.996339" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="15.282054" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="13.567768" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="11.853482" style="0" customWidth="1"/>
     <x:col min="5" max="5" width="12.567768" style="0" customWidth="1"/>
     <x:col min="6" max="6" width="11.996339" style="0" customWidth="1"/>
     <x:col min="7" max="7" width="9.853482" style="0" customWidth="1"/>
-    <x:col min="8" max="8" width="10.853482" style="0" customWidth="1"/>
+    <x:col min="8" max="8" width="9.567768" style="0" customWidth="1"/>
     <x:col min="9" max="9" width="9.853482" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:9" s="1" customFormat="1">
       <x:c r="A1" s="1" t="s">
-        <x:v>28</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="B1" s="1" t="s">
         <x:v>0</x:v>
@@ -805,7 +1346,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="D1" s="1" t="s">
-        <x:v>29</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="E1" s="1" t="s">
         <x:v>2</x:v>
@@ -821,35 +1362,6 @@
       </x:c>
       <x:c r="I1" s="1" t="s">
         <x:v>8</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2" spans="1:9">
-      <x:c r="A2" s="0" t="s">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="B2" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="C2" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="D2" s="0" t="s">
-        <x:v>31</x:v>
-      </x:c>
-      <x:c r="E2" s="0" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="F2" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="G2" s="0" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="H2" s="0" t="s">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="I2" s="0" t="s">
-        <x:v>15</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>